<commit_message>
Add two new records.
</commit_message>
<xml_diff>
--- a/original_data/Wiley_previouslyuncataloged.xlsx
+++ b/original_data/Wiley_previouslyuncataloged.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Meredith/Documents/DigitalCollections/ACWiley/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Meredith/Documents/GitHub/acwiley/original_data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{6FDF35C2-E872-734E-98D2-ECA42DC07A31}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{29510A37-1AE0-4D41-960F-478B686C1EB4}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="9360" yWindow="640" windowWidth="28040" windowHeight="17440" xr2:uid="{E3E5A948-1D07-F243-8B1D-EDC1B18C4FE8}"/>
+    <workbookView xWindow="-1180" yWindow="1700" windowWidth="28000" windowHeight="17440" xr2:uid="{E3E5A948-1D07-F243-8B1D-EDC1B18C4FE8}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="135" uniqueCount="81">
   <si>
     <t>title</t>
   </si>
@@ -217,6 +217,57 @@
   </si>
   <si>
     <t>color wheels</t>
+  </si>
+  <si>
+    <t>cw0204180</t>
+  </si>
+  <si>
+    <t>cw0204181</t>
+  </si>
+  <si>
+    <t>1909</t>
+  </si>
+  <si>
+    <t>posters</t>
+  </si>
+  <si>
+    <t>Sports in art</t>
+  </si>
+  <si>
+    <t>publisher</t>
+  </si>
+  <si>
+    <t>Norris &amp; Winter</t>
+  </si>
+  <si>
+    <t>Baseball in art</t>
+  </si>
+  <si>
+    <t>Football in art</t>
+  </si>
+  <si>
+    <t>Poster of male football player</t>
+  </si>
+  <si>
+    <t>Poster of male baseball player pitching</t>
+  </si>
+  <si>
+    <t>subject3</t>
+  </si>
+  <si>
+    <t>Tennessee Volunteers (Football team)</t>
+  </si>
+  <si>
+    <t>Tennessee Volunteers Football poster</t>
+  </si>
+  <si>
+    <t>Tennessee Volunteers Baseball poster</t>
+  </si>
+  <si>
+    <t>geographic_subject</t>
+  </si>
+  <si>
+    <t>Tennessee</t>
   </si>
 </sst>
 </file>
@@ -265,11 +316,17 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="49" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -584,28 +641,30 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BAA6A041-76A5-9744-8FAD-E7A3D2982530}">
-  <dimension ref="A1:H16"/>
+  <dimension ref="A1:K18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E5" sqref="E5"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A10" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="K26" sqref="K26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="14.83203125" customWidth="1"/>
     <col min="2" max="2" width="96.6640625" customWidth="1"/>
-    <col min="7" max="8" width="10.83203125" style="3"/>
+    <col min="3" max="3" width="36.5" style="5" customWidth="1"/>
+    <col min="7" max="7" width="11.6640625" customWidth="1"/>
+    <col min="8" max="9" width="10.83203125" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>1</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="4" t="s">
         <v>2</v>
       </c>
       <c r="D1" s="1" t="s">
@@ -615,352 +674,428 @@
         <v>4</v>
       </c>
       <c r="F1" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="G1" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="H1" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="H1" s="2" t="s">
+      <c r="I1" s="2" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="J1" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>5</v>
       </c>
       <c r="B2" t="s">
         <v>20</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C2" s="5" t="s">
         <v>21</v>
       </c>
       <c r="D2" t="s">
         <v>62</v>
       </c>
-      <c r="F2" t="s">
+      <c r="G2" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:11" ht="64" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>6</v>
       </c>
       <c r="B3" t="s">
         <v>40</v>
       </c>
-      <c r="C3" t="s">
+      <c r="C3" s="5" t="s">
         <v>55</v>
       </c>
       <c r="D3" t="s">
         <v>61</v>
       </c>
-      <c r="F3" t="s">
-        <v>60</v>
-      </c>
-      <c r="G3" s="3" t="s">
+      <c r="G3" t="s">
+        <v>60</v>
+      </c>
+      <c r="H3" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="H3" s="3" t="s">
+      <c r="I3" s="3" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:11" ht="64" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>7</v>
       </c>
       <c r="B4" t="s">
         <v>23</v>
       </c>
-      <c r="C4" t="s">
+      <c r="C4" s="5" t="s">
         <v>55</v>
       </c>
       <c r="D4" t="s">
         <v>61</v>
       </c>
-      <c r="F4" t="s">
-        <v>60</v>
-      </c>
-      <c r="G4" s="3" t="s">
+      <c r="G4" t="s">
+        <v>60</v>
+      </c>
+      <c r="H4" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="H4" s="3" t="s">
+      <c r="I4" s="3" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:11" ht="64" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>8</v>
       </c>
       <c r="B5" t="s">
         <v>41</v>
       </c>
-      <c r="C5" t="s">
+      <c r="C5" s="5" t="s">
         <v>55</v>
       </c>
       <c r="D5" t="s">
         <v>61</v>
       </c>
-      <c r="F5" t="s">
-        <v>60</v>
-      </c>
-      <c r="G5" s="3" t="s">
+      <c r="G5" t="s">
+        <v>60</v>
+      </c>
+      <c r="H5" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="H5" s="3" t="s">
+      <c r="I5" s="3" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:11" ht="64" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>9</v>
       </c>
       <c r="B6" t="s">
         <v>42</v>
       </c>
-      <c r="C6" t="s">
+      <c r="C6" s="5" t="s">
         <v>55</v>
       </c>
       <c r="D6" t="s">
         <v>61</v>
       </c>
-      <c r="F6" t="s">
-        <v>60</v>
-      </c>
-      <c r="G6" s="3" t="s">
+      <c r="G6" t="s">
+        <v>60</v>
+      </c>
+      <c r="H6" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="H6" s="3" t="s">
+      <c r="I6" s="3" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>10</v>
       </c>
       <c r="B7" t="s">
         <v>43</v>
       </c>
-      <c r="C7" t="s">
+      <c r="C7" s="5" t="s">
         <v>32</v>
       </c>
       <c r="D7" t="s">
         <v>61</v>
       </c>
-      <c r="F7" t="s">
-        <v>60</v>
-      </c>
-      <c r="G7" s="3" t="s">
+      <c r="G7" t="s">
+        <v>60</v>
+      </c>
+      <c r="H7" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="H7" s="3" t="s">
+      <c r="I7" s="3" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>11</v>
       </c>
       <c r="B8" t="s">
         <v>44</v>
       </c>
-      <c r="C8" t="s">
+      <c r="C8" s="5" t="s">
         <v>35</v>
       </c>
       <c r="D8" t="s">
         <v>61</v>
       </c>
-      <c r="F8" t="s">
-        <v>60</v>
-      </c>
-      <c r="G8" s="3" t="s">
+      <c r="G8" t="s">
+        <v>60</v>
+      </c>
+      <c r="H8" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="H8" s="3" t="s">
+      <c r="I8" s="3" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:11" ht="32" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>12</v>
       </c>
       <c r="B9" t="s">
         <v>36</v>
       </c>
-      <c r="C9" t="s">
+      <c r="C9" s="5" t="s">
         <v>37</v>
       </c>
       <c r="D9" t="s">
         <v>61</v>
       </c>
-      <c r="F9" t="s">
-        <v>60</v>
-      </c>
-      <c r="G9" s="3" t="s">
-        <v>38</v>
+      <c r="G9" t="s">
+        <v>60</v>
       </c>
       <c r="H9" s="3" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I9" s="3" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" ht="80" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>13</v>
       </c>
       <c r="B10" t="s">
         <v>39</v>
       </c>
-      <c r="C10" t="s">
+      <c r="C10" s="5" t="s">
         <v>47</v>
       </c>
       <c r="D10" t="s">
         <v>61</v>
       </c>
-      <c r="F10" t="s">
-        <v>60</v>
-      </c>
-      <c r="G10" s="3" t="s">
+      <c r="G10" t="s">
+        <v>60</v>
+      </c>
+      <c r="H10" s="3" t="s">
         <v>46</v>
       </c>
-      <c r="H10" s="3" t="s">
+      <c r="I10" s="3" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>14</v>
       </c>
       <c r="B11" t="s">
         <v>48</v>
       </c>
-      <c r="C11" t="s">
+      <c r="C11" s="5" t="s">
         <v>32</v>
       </c>
       <c r="D11" t="s">
         <v>61</v>
       </c>
-      <c r="F11" t="s">
-        <v>60</v>
-      </c>
-      <c r="G11" s="3" t="s">
+      <c r="G11" t="s">
+        <v>60</v>
+      </c>
+      <c r="H11" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="H11" s="3" t="s">
+      <c r="I11" s="3" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:11" ht="64" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>15</v>
       </c>
       <c r="B12" t="s">
         <v>40</v>
       </c>
-      <c r="C12" t="s">
+      <c r="C12" s="5" t="s">
         <v>55</v>
       </c>
       <c r="D12" t="s">
         <v>61</v>
       </c>
-      <c r="F12" t="s">
-        <v>60</v>
-      </c>
-      <c r="G12" s="3" t="s">
+      <c r="G12" t="s">
+        <v>60</v>
+      </c>
+      <c r="H12" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="H12" s="3" t="s">
+      <c r="I12" s="3" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:11" ht="64" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>16</v>
       </c>
       <c r="B13" t="s">
         <v>49</v>
       </c>
-      <c r="C13" t="s">
+      <c r="C13" s="5" t="s">
         <v>55</v>
       </c>
       <c r="D13" t="s">
         <v>61</v>
       </c>
-      <c r="F13" t="s">
-        <v>60</v>
-      </c>
-      <c r="G13" s="3" t="s">
-        <v>38</v>
+      <c r="G13" t="s">
+        <v>60</v>
       </c>
       <c r="H13" s="3" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I13" s="3" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" ht="32" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>17</v>
       </c>
       <c r="B14" t="s">
         <v>50</v>
       </c>
-      <c r="C14" t="s">
+      <c r="C14" s="5" t="s">
         <v>53</v>
       </c>
       <c r="D14" t="s">
         <v>61</v>
       </c>
-      <c r="F14" t="s">
-        <v>60</v>
-      </c>
-      <c r="G14" s="3" t="s">
+      <c r="G14" t="s">
+        <v>60</v>
+      </c>
+      <c r="H14" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="H14" s="3" t="s">
+      <c r="I14" s="3" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:11" ht="32" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>18</v>
       </c>
       <c r="B15" t="s">
         <v>54</v>
       </c>
-      <c r="C15" t="s">
+      <c r="C15" s="5" t="s">
         <v>56</v>
       </c>
       <c r="D15" t="s">
         <v>61</v>
       </c>
-      <c r="F15" t="s">
-        <v>60</v>
-      </c>
-      <c r="G15" s="3" t="s">
+      <c r="G15" t="s">
+        <v>60</v>
+      </c>
+      <c r="H15" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="H15" s="3" t="s">
+      <c r="I15" s="3" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:11" ht="64" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>19</v>
       </c>
       <c r="B16" t="s">
         <v>57</v>
       </c>
-      <c r="C16" t="s">
+      <c r="C16" s="5" t="s">
         <v>55</v>
       </c>
       <c r="D16" t="s">
         <v>61</v>
       </c>
-      <c r="F16" t="s">
-        <v>60</v>
-      </c>
-      <c r="G16" s="3" t="s">
+      <c r="G16" t="s">
+        <v>60</v>
+      </c>
+      <c r="H16" s="3" t="s">
         <v>58</v>
       </c>
-      <c r="H16" s="3" t="s">
+      <c r="I16" s="3" t="s">
         <v>59</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
+        <v>64</v>
+      </c>
+      <c r="B17" t="s">
+        <v>77</v>
+      </c>
+      <c r="C17" s="5" t="s">
+        <v>73</v>
+      </c>
+      <c r="D17" t="s">
+        <v>68</v>
+      </c>
+      <c r="E17" t="s">
+        <v>72</v>
+      </c>
+      <c r="G17" t="s">
+        <v>67</v>
+      </c>
+      <c r="H17" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="I17" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="J17" t="s">
+        <v>70</v>
+      </c>
+      <c r="K17" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
+        <v>65</v>
+      </c>
+      <c r="B18" t="s">
+        <v>78</v>
+      </c>
+      <c r="C18" s="5" t="s">
+        <v>74</v>
+      </c>
+      <c r="D18" t="s">
+        <v>68</v>
+      </c>
+      <c r="E18" t="s">
+        <v>71</v>
+      </c>
+      <c r="F18" t="s">
+        <v>76</v>
+      </c>
+      <c r="G18" t="s">
+        <v>67</v>
+      </c>
+      <c r="H18" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="I18" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="J18" t="s">
+        <v>70</v>
+      </c>
+      <c r="K18" t="s">
+        <v>80</v>
       </c>
     </row>
   </sheetData>

</xml_diff>